<commit_message>
wav file load py code
</commit_message>
<xml_diff>
--- a/Project/02. Prepreocessing/특정부위별 데이터 분류.xlsx
+++ b/Project/02. Prepreocessing/특정부위별 데이터 분류.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이상민\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\국제문화대학\Desktop\AI_Project\Project\02. Prepreocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D627AF4C-51F7-4B15-8042-2D0D76D5142E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="10590" xr2:uid="{6CEE3C3C-7660-41E1-AB99-2459E7AD3063}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,30 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$65</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{7AD08BE1-8E67-4560-84E8-54591FB03DE0}" keepAlive="1" name="쿼리 - pop" description="통합 문서의 'pop' 쿼리에 대한 연결입니다." type="5" refreshedVersion="6" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="쿼리 - pop" description="통합 문서의 'pop' 쿼리에 대한 연결입니다." type="5" refreshedVersion="6" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=pop;Extended Properties=&quot;&quot;" command="SELECT * FROM [pop]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="213">
   <si>
     <t>번호</t>
   </si>
@@ -126,12 +120,576 @@
   <si>
     <t>질병</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>101_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>102_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>104_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>105_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>108_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>109_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>110_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>110_1p1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>110_1p1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>110_1p1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>110_1p1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>111_1b2_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>111_1b3_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>112_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>112_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>112_1p1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>112_1p1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>112_1p1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>113_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>115_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>116_1b2_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>116_1b2_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>118_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>119_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>120_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>120_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>120_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>120_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>120_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>121_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>121_1p1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>123_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>124_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>125_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>126_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>127_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>129_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>131_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>136_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>137_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>137_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>139_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>143_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>144_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>144_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>148_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>149_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>149_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>149_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>150_1b2_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>152_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>153_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>157_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>157_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>157_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>157_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>157_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>159_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>159_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>159_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>159_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>161_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>161_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>164_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>165_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>165_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>165_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>166_1p1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>166_1p1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>166_1p1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>166_1p1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>166_1p1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>167_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>167_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>168_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>169_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>169_1b2_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>171_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>173_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>175_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>179_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>179_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>182_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>183_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>183_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>184_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>185_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>187_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>188_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>188_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>188_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>188_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>190_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>194_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>194_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Al_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Ll_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Lr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>195_1b1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>196_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>197_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>197_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b2_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b2_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b3_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>201_1b3_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>202_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>206_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>206_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>206_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>208_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>209_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>210_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>210_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>214_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>215_1b2_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>215_1b3_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>216_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>216_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>217_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>218_1p1_Ar_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>218_1p1_Pl_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>218_1p1_Pr_sc_Litt3200.wav</t>
+  </si>
+  <si>
+    <t>222_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>222_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>222_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Ar_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Lr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>223_1b1_Pr_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>224_1b1_Tc_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>224_1b2_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>225_1b1_Pl_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>226_1b1_Al_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>226_1b1_Ll_sc_Meditron.wav</t>
+  </si>
+  <si>
+    <t>226_1b1_Pl_sc_LittC2SE.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +729,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -488,11 +1049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E34C295-58E6-4E32-A6F2-01370D450F32}">
-  <dimension ref="A1:J66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -500,7 +1061,7 @@
     <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -549,8 +1110,15 @@
         <f>COUNTIF(C2:I2,"O")</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" t="str">
+        <f>LEFT(M2,3)</f>
+        <v>101</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>104</v>
       </c>
@@ -579,8 +1147,15 @@
         <f t="shared" ref="J3:J65" si="0">COUNTIF(C3:I3,"O")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="1" t="str">
+        <f t="shared" ref="L3:L66" si="1">LEFT(M3,3)</f>
+        <v>101</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>105</v>
       </c>
@@ -594,8 +1169,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>108</v>
       </c>
@@ -612,8 +1194,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>109</v>
       </c>
@@ -642,8 +1231,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>110</v>
       </c>
@@ -669,8 +1265,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>111</v>
       </c>
@@ -684,8 +1287,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>112</v>
       </c>
@@ -708,8 +1318,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>113</v>
       </c>
@@ -738,8 +1355,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>116</v>
       </c>
@@ -756,8 +1380,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>118</v>
       </c>
@@ -786,8 +1417,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>120</v>
       </c>
@@ -813,8 +1451,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>121</v>
       </c>
@@ -828,8 +1473,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>123</v>
       </c>
@@ -846,8 +1498,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>124</v>
       </c>
@@ -876,8 +1535,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>125</v>
       </c>
@@ -891,8 +1557,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>126</v>
       </c>
@@ -909,8 +1582,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>131</v>
       </c>
@@ -927,8 +1607,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>137</v>
       </c>
@@ -942,8 +1629,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>139</v>
       </c>
@@ -972,8 +1666,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>143</v>
       </c>
@@ -990,8 +1691,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>144</v>
       </c>
@@ -1011,8 +1719,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>148</v>
       </c>
@@ -1029,8 +1744,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>149</v>
       </c>
@@ -1053,8 +1775,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>150</v>
       </c>
@@ -1071,8 +1800,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>152</v>
       </c>
@@ -1089,8 +1825,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>153</v>
       </c>
@@ -1107,8 +1850,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>157</v>
       </c>
@@ -1134,8 +1884,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>159</v>
       </c>
@@ -1158,8 +1915,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>161</v>
       </c>
@@ -1179,8 +1943,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>164</v>
       </c>
@@ -1194,8 +1965,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>165</v>
       </c>
@@ -1212,8 +1990,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>166</v>
       </c>
@@ -1239,8 +2024,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>167</v>
       </c>
@@ -1260,8 +2052,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>168</v>
       </c>
@@ -1278,8 +2077,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>169</v>
       </c>
@@ -1296,8 +2102,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>171</v>
       </c>
@@ -1314,8 +2127,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>173</v>
       </c>
@@ -1332,8 +2152,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>175</v>
       </c>
@@ -1362,8 +2189,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>179</v>
       </c>
@@ -1383,8 +2217,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>182</v>
       </c>
@@ -1398,8 +2239,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>183</v>
       </c>
@@ -1416,8 +2264,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>185</v>
       </c>
@@ -1446,8 +2301,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>187</v>
       </c>
@@ -1461,8 +2323,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>188</v>
       </c>
@@ -1485,8 +2354,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>190</v>
       </c>
@@ -1500,8 +2376,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L47" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>194</v>
       </c>
@@ -1518,8 +2401,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L48" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>195</v>
       </c>
@@ -1548,8 +2438,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L49" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>196</v>
       </c>
@@ -1563,8 +2460,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L50" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>197</v>
       </c>
@@ -1584,8 +2488,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L51" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>201</v>
       </c>
@@ -1602,8 +2513,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L52" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>206</v>
       </c>
@@ -1620,8 +2538,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>208</v>
       </c>
@@ -1635,8 +2560,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>209</v>
       </c>
@@ -1650,8 +2582,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>210</v>
       </c>
@@ -1668,8 +2607,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L56" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>215</v>
       </c>
@@ -1683,8 +2629,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L57" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>216</v>
       </c>
@@ -1704,8 +2657,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>217</v>
       </c>
@@ -1719,8 +2679,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L59" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>218</v>
       </c>
@@ -1746,8 +2713,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>222</v>
       </c>
@@ -1764,8 +2738,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L61" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>223</v>
       </c>
@@ -1794,8 +2775,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>224</v>
       </c>
@@ -1815,8 +2803,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L63" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>225</v>
       </c>
@@ -1830,8 +2825,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L64" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>226</v>
       </c>
@@ -1854,21 +2856,1143 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L65" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J66">
         <f>SUM(J2:J65)</f>
         <v>186</v>
       </c>
+      <c r="L66" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L67" s="1" t="str">
+        <f t="shared" ref="L67:L130" si="2">LEFT(M67,3)</f>
+        <v>137</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L68" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L69" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L70" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L71" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L72" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L73" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L74" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L75" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L76" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L77" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L78" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L79" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L80" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L81" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L82" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L83" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L84" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L85" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="86" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L86" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L87" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L88" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L89" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L90" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L91" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L92" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L93" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L94" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="95" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L95" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L96" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L97" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L98" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="99" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L99" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L100" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L101" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L102" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L103" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L104" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="105" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L105" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="106" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L106" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="107" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L107" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="108" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L108" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L109" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="110" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L110" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="111" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L111" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="112" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L112" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="113" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L113" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="114" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L114" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L115" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="116" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L116" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="117" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L117" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="118" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L118" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="119" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L119" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="120" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L120" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="121" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L121" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="122" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L122" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="123" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L123" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="124" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L124" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="125" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L125" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="126" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L126" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="127" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L127" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L128" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L129" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="130" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L130" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="131" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L131" s="1" t="str">
+        <f t="shared" ref="L131:L189" si="3">LEFT(M131,3)</f>
+        <v>188</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="132" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L132" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="133" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L133" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="134" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L134" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="135" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L135" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="136" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L136" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="137" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L137" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="138" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L138" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="139" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L139" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="140" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L140" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="141" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L141" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="142" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L142" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="143" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L143" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="144" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L144" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="145" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L145" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="146" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L146" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="147" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L147" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="148" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L148" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="149" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L149" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="150" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L150" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="151" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L151" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="152" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L152" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="153" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L153" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="154" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L154" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="155" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L155" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="156" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L156" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="157" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L157" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="158" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L158" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="159" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L159" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="160" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L160" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="M160" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="161" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L161" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>214</v>
+      </c>
+      <c r="M161" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="162" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L162" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>215</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="163" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L163" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>215</v>
+      </c>
+      <c r="M163" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="164" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L164" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>216</v>
+      </c>
+      <c r="M164" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="165" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L165" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>216</v>
+      </c>
+      <c r="M165" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="166" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L166" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>217</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="167" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L167" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M167" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="168" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L168" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M168" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="169" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L169" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M169" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="170" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L170" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M170" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="171" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L171" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="172" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L172" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M172" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="173" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L173" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M173" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="174" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L174" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="175" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L175" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>222</v>
+      </c>
+      <c r="M175" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L176" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>222</v>
+      </c>
+      <c r="M176" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="177" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L177" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>222</v>
+      </c>
+      <c r="M177" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="178" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L178" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M178" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="179" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L179" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M179" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="180" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L180" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M180" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="181" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L181" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M181" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="182" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L182" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M182" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="183" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L183" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="M183" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="184" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L184" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>224</v>
+      </c>
+      <c r="M184" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="185" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L185" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>224</v>
+      </c>
+      <c r="M185" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="186" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L186" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="M186" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="187" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L187" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
+      <c r="M187" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="188" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L188" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
+      <c r="M188" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="189" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L189" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
+      <c r="M189" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FDE00D-4A11-41AE-A2CF-065817FF5D53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
@@ -1933,7 +4057,7 @@
         <v>O</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:H2" si="0">IF(MATCH($A2,K$2:K$44,)&gt;0, "O")</f>
+        <f t="shared" ref="C2" si="0">IF(MATCH($A2,K$2:K$44,)&gt;0, "O")</f>
         <v>O</v>
       </c>
       <c r="D2" t="e">
@@ -2037,7 +4161,7 @@
         <v>104</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B3:B66" si="12">IF(MATCH(A4,$J$2:$J$44,)&gt;0, "O")</f>
+        <f t="shared" ref="B4:B66" si="12">IF(MATCH(A4,$J$2:$J$44,)&gt;0, "O")</f>
         <v>O</v>
       </c>
       <c r="C4" t="str">

</xml_diff>